<commit_message>
trying the push again
</commit_message>
<xml_diff>
--- a/data/schoolchoicepopularity_education_next/EdNext_SchoolChoice (Autosaved)2.xlsx
+++ b/data/schoolchoicepopularity_education_next/EdNext_SchoolChoice (Autosaved)2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6816" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6816" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Public Opinion on Charter Schools</t>
   </si>
@@ -1280,11 +1280,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="288033816"/>
-        <c:axId val="288039696"/>
+        <c:axId val="524720584"/>
+        <c:axId val="524717056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="288033816"/>
+        <c:axId val="524720584"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1327,7 +1327,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288039696"/>
+        <c:crossAx val="524717056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1335,7 +1335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288039696"/>
+        <c:axId val="524717056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1387,7 +1387,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288033816"/>
+        <c:crossAx val="524720584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1478,660 +1478,6 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Support for</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Charter Schools By Political Party</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.11928563270556694"/>
-          <c:y val="8.0672994332476516E-2"/>
-          <c:w val="0.85985842546515256"/>
-          <c:h val="0.69628613157660901"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018 only'!$C$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$25:$B$30</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2018 only'!$C$25:$C$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018 only'!$D$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$25:$B$30</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2018 only'!$D$25:$D$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018 only'!$E$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$25:$B$30</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2018 only'!$E$25:$E$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018 only'!$F$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$25:$B$30</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2018 only'!$F$25:$F$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018 only'!$G$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$25:$B$30</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2018 only'!$G$25:$G$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="288035384"/>
-        <c:axId val="288036560"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="288035384"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="288036560"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="288036560"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="288035384"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2795,11 +2141,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="289646720"/>
-        <c:axId val="289648680"/>
+        <c:axId val="524719016"/>
+        <c:axId val="524717840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="289646720"/>
+        <c:axId val="524719016"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2839,7 +2185,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289648680"/>
+        <c:crossAx val="524717840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2847,7 +2193,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="289648680"/>
+        <c:axId val="524717840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2899,7 +2245,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289646720"/>
+        <c:crossAx val="524719016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2948,7 +2294,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3348,11 +2694,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="173192920"/>
-        <c:axId val="288041264"/>
+        <c:axId val="524719408"/>
+        <c:axId val="524718624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173192920"/>
+        <c:axId val="524719408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3395,7 +2741,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288041264"/>
+        <c:crossAx val="524718624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3403,7 +2749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288041264"/>
+        <c:axId val="524718624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3512,7 +2858,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173192920"/>
+        <c:crossAx val="524719408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3596,7 +2942,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3638,7 +2984,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3911,11 +3256,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="288037344"/>
-        <c:axId val="288036168"/>
+        <c:axId val="232927312"/>
+        <c:axId val="232923000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288037344"/>
+        <c:axId val="232927312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3958,7 +3303,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288036168"/>
+        <c:crossAx val="232923000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3966,7 +3311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288036168"/>
+        <c:axId val="232923000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4017,7 +3362,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288037344"/>
+        <c:crossAx val="232927312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4031,7 +3376,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4098,7 +3442,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4140,7 +3484,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4498,11 +3841,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="288034600"/>
-        <c:axId val="288036952"/>
+        <c:axId val="232928096"/>
+        <c:axId val="232924176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288034600"/>
+        <c:axId val="232928096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4545,7 +3888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288036952"/>
+        <c:crossAx val="232924176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4553,7 +3896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288036952"/>
+        <c:axId val="232924176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4601,7 +3944,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4662,7 +4004,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288034600"/>
+        <c:crossAx val="232928096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4680,7 +4022,6 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4746,7 +4087,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5060,11 +4401,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="288035776"/>
-        <c:axId val="288037736"/>
+        <c:axId val="232927704"/>
+        <c:axId val="232922216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288035776"/>
+        <c:axId val="232927704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5107,7 +4448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288037736"/>
+        <c:crossAx val="232922216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5115,7 +4456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288037736"/>
+        <c:axId val="232922216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -5222,7 +4563,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288035776"/>
+        <c:crossAx val="232927704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5302,7 +4643,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5862,11 +5203,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="288040088"/>
-        <c:axId val="288040872"/>
+        <c:axId val="232923784"/>
+        <c:axId val="232924960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288040088"/>
+        <c:axId val="232923784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5909,7 +5250,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288040872"/>
+        <c:crossAx val="232924960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5917,7 +5258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288040872"/>
+        <c:axId val="232924960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6025,7 +5366,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288040088"/>
+        <c:crossAx val="232923784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6387,46 +5728,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -7438,7 +6739,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7546,6 +6847,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -7556,6 +6862,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -7587,6 +6898,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7642,23 +6956,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -7763,8 +7076,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7896,20 +7209,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -9491,522 +8803,6 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10556,36 +9352,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>331303</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>84113</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>406450</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>30426</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>70180</xdr:colOff>
       <xdr:row>46</xdr:row>
@@ -10608,7 +9374,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11166,8 +9932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView zoomScale="36" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" zoomScale="36" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="T50" sqref="T50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11483,125 +10249,95 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="24" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>26</v>
-      </c>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>6</v>
-      </c>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>7</v>
-      </c>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>8</v>
-      </c>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
     </row>
     <row r="35" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -11706,7 +10442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="103" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
backing up a file version so that I can leave the master (github is angry that this file isn't backed up ,but it's not an important file
</commit_message>
<xml_diff>
--- a/data/schoolchoicepopularity_education_next/EdNext_SchoolChoice (Autosaved)2.xlsx
+++ b/data/schoolchoicepopularity_education_next/EdNext_SchoolChoice (Autosaved)2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6816" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6816" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Public Opinion on Charter Schools</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>TOTAL strong or somewhat support</t>
-  </si>
-  <si>
-    <t>hi</t>
   </si>
 </sst>
 </file>
@@ -1280,11 +1277,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="288033816"/>
-        <c:axId val="288039696"/>
+        <c:axId val="524720584"/>
+        <c:axId val="524717056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="288033816"/>
+        <c:axId val="524720584"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1327,7 +1324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288039696"/>
+        <c:crossAx val="524717056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1335,7 +1332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288039696"/>
+        <c:axId val="524717056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1387,7 +1384,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288033816"/>
+        <c:crossAx val="524720584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1478,660 +1475,6 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Support for</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Charter Schools By Political Party</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.11928563270556694"/>
-          <c:y val="8.0672994332476516E-2"/>
-          <c:w val="0.85985842546515256"/>
-          <c:h val="0.69628613157660901"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018 only'!$C$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$25:$B$30</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2018 only'!$C$25:$C$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018 only'!$D$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$25:$B$30</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2018 only'!$D$25:$D$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018 only'!$E$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$25:$B$30</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2018 only'!$E$25:$E$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018 only'!$F$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$25:$B$30</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2018 only'!$F$25:$F$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018 only'!$G$24</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'2018 only'!$A$25:$B$30</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Republicans</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Democrats</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Teachers</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2018 only'!$G$25:$G$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="288035384"/>
-        <c:axId val="288036560"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="288035384"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="288036560"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="288036560"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="288035384"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2795,11 +2138,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="289646720"/>
-        <c:axId val="289648680"/>
+        <c:axId val="524719016"/>
+        <c:axId val="524717840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="289646720"/>
+        <c:axId val="524719016"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2839,7 +2182,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289648680"/>
+        <c:crossAx val="524717840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2847,7 +2190,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="289648680"/>
+        <c:axId val="524717840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2899,7 +2242,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="289646720"/>
+        <c:crossAx val="524719016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2948,7 +2291,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3348,11 +2691,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="173192920"/>
-        <c:axId val="288041264"/>
+        <c:axId val="524719408"/>
+        <c:axId val="524718624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="173192920"/>
+        <c:axId val="524719408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3395,7 +2738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288041264"/>
+        <c:crossAx val="524718624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3403,7 +2746,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288041264"/>
+        <c:axId val="524718624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3512,7 +2855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="173192920"/>
+        <c:crossAx val="524719408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3596,7 +2939,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3638,7 +2981,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3911,11 +3253,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="288037344"/>
-        <c:axId val="288036168"/>
+        <c:axId val="232927312"/>
+        <c:axId val="232923000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288037344"/>
+        <c:axId val="232927312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3958,7 +3300,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288036168"/>
+        <c:crossAx val="232923000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3966,7 +3308,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288036168"/>
+        <c:axId val="232923000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4017,7 +3359,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288037344"/>
+        <c:crossAx val="232927312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4031,7 +3373,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4098,7 +3439,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4140,7 +3481,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4498,11 +3838,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="288034600"/>
-        <c:axId val="288036952"/>
+        <c:axId val="232928096"/>
+        <c:axId val="232924176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288034600"/>
+        <c:axId val="232928096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4545,7 +3885,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288036952"/>
+        <c:crossAx val="232924176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4553,7 +3893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288036952"/>
+        <c:axId val="232924176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4601,7 +3941,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4662,7 +4001,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288034600"/>
+        <c:crossAx val="232928096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4680,7 +4019,6 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4746,7 +4084,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5060,11 +4398,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="288035776"/>
-        <c:axId val="288037736"/>
+        <c:axId val="232927704"/>
+        <c:axId val="232922216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288035776"/>
+        <c:axId val="232927704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5107,7 +4445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288037736"/>
+        <c:crossAx val="232922216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5115,7 +4453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288037736"/>
+        <c:axId val="232922216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -5222,7 +4560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288035776"/>
+        <c:crossAx val="232927704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5302,7 +4640,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5862,11 +5200,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="288040088"/>
-        <c:axId val="288040872"/>
+        <c:axId val="232923784"/>
+        <c:axId val="232924960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="288040088"/>
+        <c:axId val="232923784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5909,7 +5247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288040872"/>
+        <c:crossAx val="232924960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5917,7 +5255,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="288040872"/>
+        <c:axId val="232924960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6025,7 +5363,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288040088"/>
+        <c:crossAx val="232923784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6387,46 +5725,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -7438,7 +6736,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7546,6 +6844,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -7556,6 +6859,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -7587,6 +6895,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7642,23 +6953,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -7763,8 +7073,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7896,20 +7206,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -9491,522 +8800,6 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10556,36 +9349,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>331303</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>84113</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>406450</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>30426</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>70180</xdr:colOff>
       <xdr:row>46</xdr:row>
@@ -10608,7 +9371,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11164,10 +9927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView zoomScale="36" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" zoomScale="14" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11483,128 +10246,98 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="24" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>26</v>
-      </c>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>6</v>
-      </c>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>7</v>
-      </c>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>8</v>
-      </c>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
     </row>
-    <row r="35" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="35" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="24" t="s">
         <v>23</v>
       </c>
@@ -11628,7 +10361,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="16"/>
       <c r="B37" s="7" t="s">
         <v>6</v>
@@ -11653,7 +10386,7 @@
         <v>0.57000000000000006</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="38" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A38" s="19"/>
       <c r="B38" s="20" t="s">
         <v>7</v>
@@ -11676,23 +10409,6 @@
       <c r="H38" s="31">
         <f>SUM(C38:D38)</f>
         <v>0.36000000000000004</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="I42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="10:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="J74">
-        <f>12+33</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="75" spans="10:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="J75">
-        <f>16+30</f>
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -11706,7 +10422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="103" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>